<commit_message>
doing some justice again
</commit_message>
<xml_diff>
--- a/assets/import/contoh.xlsx
+++ b/assets/import/contoh.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>NIS LOKAL</t>
   </si>
@@ -44,12 +44,6 @@
     <t>TEMPAT LAHIR</t>
   </si>
   <si>
-    <t>TANGGAL LAHIR</t>
-  </si>
-  <si>
-    <t>JENIS KELAMIN</t>
-  </si>
-  <si>
     <t>ALAMAT LENGKAP</t>
   </si>
   <si>
@@ -153,6 +147,15 @@
   </si>
   <si>
     <t>KELAS PONDOK</t>
+  </si>
+  <si>
+    <t>JUMLAH SAUDARA</t>
+  </si>
+  <si>
+    <t>JENIS KELAMIN (L / P)</t>
+  </si>
+  <si>
+    <t>TANGGAL LAHIR (tt-BB-TTTT)</t>
   </si>
 </sst>
 </file>
@@ -499,10 +502,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AQ4"/>
+  <dimension ref="A1:AR2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AL1" workbookViewId="0">
-      <selection activeCell="AQ1" sqref="AQ1"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1:M1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -511,12 +514,21 @@
     <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="14.28515625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="14" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="22.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -536,508 +548,252 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="W1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="X1" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="Y1" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="Z1" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="AA1" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="3" t="s">
+      <c r="AB1" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AC1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AD1" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="3" t="s">
+      <c r="AE1" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="AD1" s="3" t="s">
+      <c r="AF1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="AE1" s="3" t="s">
+      <c r="AG1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="AF1" s="3" t="s">
+      <c r="AH1" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="AG1" s="4" t="s">
+      <c r="AI1" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="AH1" s="4" t="s">
+      <c r="AJ1" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="AI1" s="4" t="s">
+      <c r="AK1" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="AJ1" s="4" t="s">
+      <c r="AL1" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="AM1" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="AK1" s="4" t="s">
+      <c r="AN1" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="AL1" s="4" t="s">
+      <c r="AO1" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="AM1" s="4" t="s">
+      <c r="AP1" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="AN1" s="4" t="s">
+      <c r="AQ1" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="AO1" s="4" t="s">
+      <c r="AR1" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="AP1" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="AQ1" s="4" t="s">
-        <v>42</v>
-      </c>
     </row>
-    <row r="2" spans="1:43" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:44" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>987</v>
+        <v>0</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="M2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="N2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="R2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="S2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="T2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="U2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="V2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="X2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AH2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AI2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AP2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AQ2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>144</v>
-      </c>
-      <c r="B3">
-        <v>1321231</v>
-      </c>
-      <c r="C3">
-        <v>1321231</v>
-      </c>
-      <c r="D3">
-        <v>1321231</v>
-      </c>
-      <c r="E3">
-        <v>1321231</v>
-      </c>
-      <c r="F3">
-        <v>1321231</v>
-      </c>
-      <c r="G3">
-        <v>1321231</v>
-      </c>
-      <c r="H3">
-        <v>1321231</v>
-      </c>
-      <c r="I3">
-        <v>1321231</v>
-      </c>
-      <c r="J3">
-        <v>1321231</v>
-      </c>
-      <c r="K3">
-        <v>1321231</v>
-      </c>
-      <c r="L3">
-        <v>1321231</v>
-      </c>
-      <c r="M3">
-        <v>1321231</v>
-      </c>
-      <c r="N3">
-        <v>1321231</v>
-      </c>
-      <c r="O3">
-        <v>1321231</v>
-      </c>
-      <c r="P3">
-        <v>1321231</v>
-      </c>
-      <c r="Q3">
-        <v>1321231</v>
-      </c>
-      <c r="R3">
-        <v>1321231</v>
-      </c>
-      <c r="S3">
-        <v>1321231</v>
-      </c>
-      <c r="T3">
-        <v>1321231</v>
-      </c>
-      <c r="U3">
-        <v>1321231</v>
-      </c>
-      <c r="V3">
-        <v>1321231</v>
-      </c>
-      <c r="W3">
-        <v>1321231</v>
-      </c>
-      <c r="X3">
-        <v>1321231</v>
-      </c>
-      <c r="Y3">
-        <v>1321231</v>
-      </c>
-      <c r="Z3">
-        <v>1321231</v>
-      </c>
-      <c r="AA3">
-        <v>1321231</v>
-      </c>
-      <c r="AB3">
-        <v>1321231</v>
-      </c>
-      <c r="AC3">
-        <v>1321231</v>
-      </c>
-      <c r="AD3">
-        <v>1321231</v>
-      </c>
-      <c r="AE3">
-        <v>1321231</v>
-      </c>
-      <c r="AF3">
-        <v>1321231</v>
-      </c>
-      <c r="AG3">
-        <v>1321231</v>
-      </c>
-      <c r="AH3">
-        <v>1321231</v>
-      </c>
-      <c r="AI3">
-        <v>1321231</v>
-      </c>
-      <c r="AJ3">
-        <v>1321231</v>
-      </c>
-      <c r="AK3">
-        <v>1321231</v>
-      </c>
-      <c r="AL3">
-        <v>1321231</v>
-      </c>
-      <c r="AM3">
-        <v>1321231</v>
-      </c>
-      <c r="AN3">
-        <v>1321231</v>
-      </c>
-      <c r="AO3">
-        <v>1321231</v>
-      </c>
-      <c r="AP3">
-        <v>1321231</v>
-      </c>
-      <c r="AQ3">
-        <v>1321231</v>
-      </c>
-    </row>
-    <row r="4" spans="1:43" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>1113</v>
-      </c>
-      <c r="B4">
-        <v>1113</v>
-      </c>
-      <c r="C4">
-        <v>1113</v>
-      </c>
-      <c r="D4">
-        <v>1113</v>
-      </c>
-      <c r="E4">
-        <v>1113</v>
-      </c>
-      <c r="F4">
-        <v>1113</v>
-      </c>
-      <c r="G4">
-        <v>1113</v>
-      </c>
-      <c r="H4">
-        <v>1113</v>
-      </c>
-      <c r="I4">
-        <v>1113</v>
-      </c>
-      <c r="J4">
-        <v>1113</v>
-      </c>
-      <c r="K4">
-        <v>1113</v>
-      </c>
-      <c r="L4">
-        <v>1113</v>
-      </c>
-      <c r="M4">
-        <v>1113</v>
-      </c>
-      <c r="N4">
-        <v>1113</v>
-      </c>
-      <c r="O4">
-        <v>1113</v>
-      </c>
-      <c r="P4">
-        <v>1113</v>
-      </c>
-      <c r="Q4">
-        <v>1113</v>
-      </c>
-      <c r="R4">
-        <v>1113</v>
-      </c>
-      <c r="S4">
-        <v>1113</v>
-      </c>
-      <c r="T4">
-        <v>1113</v>
-      </c>
-      <c r="U4">
-        <v>1113</v>
-      </c>
-      <c r="V4">
-        <v>1113</v>
-      </c>
-      <c r="W4">
-        <v>1113</v>
-      </c>
-      <c r="X4">
-        <v>1113</v>
-      </c>
-      <c r="Y4">
-        <v>1113</v>
-      </c>
-      <c r="Z4">
-        <v>1113</v>
-      </c>
-      <c r="AA4">
-        <v>1113</v>
-      </c>
-      <c r="AB4">
-        <v>1113</v>
-      </c>
-      <c r="AC4">
-        <v>1113</v>
-      </c>
-      <c r="AD4">
-        <v>1113</v>
-      </c>
-      <c r="AE4">
-        <v>1113</v>
-      </c>
-      <c r="AF4">
-        <v>1113</v>
-      </c>
-      <c r="AG4">
-        <v>1113</v>
-      </c>
-      <c r="AH4">
-        <v>1113</v>
-      </c>
-      <c r="AI4">
-        <v>1113</v>
-      </c>
-      <c r="AJ4">
-        <v>1113</v>
-      </c>
-      <c r="AK4">
-        <v>1113</v>
-      </c>
-      <c r="AL4">
-        <v>1113</v>
-      </c>
-      <c r="AM4">
-        <v>1113</v>
-      </c>
-      <c r="AN4">
-        <v>1113</v>
-      </c>
-      <c r="AO4">
-        <v>1113</v>
-      </c>
-      <c r="AP4">
-        <v>1113</v>
-      </c>
-      <c r="AQ4">
-        <v>1113</v>
+        <v>0</v>
+      </c>
+      <c r="AR2">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>